<commit_message>
Updates and spreadsheet added
</commit_message>
<xml_diff>
--- a/TestData/rates.xlsx
+++ b/TestData/rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tokyomanamela/git/APIAutomation/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thaboramalitse/git/APIAutomation/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943EBC4C-C2D3-CB42-874A-E4A19F786EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B37B1D-F26A-DA46-A515-563F2B18171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{C803A493-06B4-7442-A1DD-EE01984397FF}"/>
+    <workbookView xWindow="760" yWindow="400" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{C803A493-06B4-7442-A1DD-EE01984397FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -151,9 +151,6 @@
     <t>ChildPremiumAmount7_5K</t>
   </si>
   <si>
-    <t>ChildPremiumAmount17_5K</t>
-  </si>
-  <si>
     <t>ParentPremiumAmount10K</t>
   </si>
   <si>
@@ -172,17 +169,47 @@
     <t>MainLife</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>196.0</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>49.0</t>
+  </si>
+  <si>
     <t>110.0</t>
   </si>
   <si>
     <t>136.0</t>
+  </si>
+  <si>
+    <t>162.0</t>
+  </si>
+  <si>
+    <t>214.0</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>ChildPremiumAmount15K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,6 +230,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -231,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -240,6 +273,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +591,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,7 +659,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
@@ -669,10 +703,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -713,10 +747,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -765,7 +799,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,16 +883,16 @@
         <v>34</v>
       </c>
       <c r="R1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="S1" t="s">
         <v>35</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
@@ -866,19 +900,64 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>60100000</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
         <v>46</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>